<commit_message>
correct chronology for P051
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_reassigned_chronology.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_reassigned_chronology.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816B7291-6AEE-0049-9ED6-C6D6CF0E7F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A118FC9-ACCA-F448-8FB9-F3E3C671F53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16060" xr2:uid="{55831CDA-BA01-2F47-B5CB-31B623A29375}"/>
   </bookViews>
@@ -839,7 +839,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1116,13 +1116,13 @@
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
change Chinese phase for P052 and P053
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_reassigned_chronology.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_reassigned_chronology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A118FC9-ACCA-F448-8FB9-F3E3C671F53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1640BAC8-04C6-754F-8E23-23075B632DDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16060" xr2:uid="{55831CDA-BA01-2F47-B5CB-31B623A29375}"/>
   </bookViews>
@@ -839,7 +839,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,7 +1166,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
@@ -1234,7 +1234,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>27</v>
@@ -1305,7 +1305,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>27</v>
@@ -1361,7 +1361,7 @@
         <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>27</v>
@@ -1417,7 +1417,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>27</v>

</xml_diff>